<commit_message>
Major reorganization to reduce future editing.
</commit_message>
<xml_diff>
--- a/Object Resource Numbers.xlsx
+++ b/Object Resource Numbers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="-20" windowWidth="23160" windowHeight="17900" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="-20" windowWidth="24960" windowHeight="19220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Object Resource Numbers.txt" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="231">
+  <si>
+    <t>provides the logical complement of a number or a list of numbers, returning '0' for each non-zero number and '1' for each zero number</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>an implementation of the APL 'reduction' operator, which is used to apply an operator over the elements of a vector</t>
+  </si>
+  <si>
+    <t>redirects a bang to a randomly selected outlet</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
   <si>
     <t>Y</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -29,14 +43,315 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>an implementation of the APL 'reverse' operator, which is used to reverse the order of the elements of a vector</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>an interface to the serial ports on a Macintosh; use standard 'serial' object for Max 4.3+</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>[not distributed]</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[not built, doPlügin variant] </t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>(sublist matching)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of objects defined</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of objects still to be done</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of objects implemented</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>an implementation of the APL 'rotate' operator, which is used to rotate the elements of a vector</t>
+  </si>
+  <si>
+    <t>calculates the integer nearest to the value given</t>
+  </si>
+  <si>
+    <t>removes 'noise' numbers from the end of a list</t>
+  </si>
+  <si>
+    <t>an implementation of the APL 'scan' operator, which is used to apply an operator over the elements of a vector</t>
+  </si>
+  <si>
+    <t>extracts a portion of a list</t>
+  </si>
+  <si>
+    <t>calculates the sine of the input</t>
+  </si>
+  <si>
+    <t>a combination of Vdrop and Vtake</t>
+  </si>
+  <si>
+    <t>calculates the square root of the input</t>
+  </si>
+  <si>
+    <t>an implementation of the APL 'take' operator, which is used to return leading or trailing elements of a vector</t>
+  </si>
+  <si>
+    <t>partitions a list of numbers into a sequence of sublists, separated by 'noise' numbers in the original list</t>
+  </si>
+  <si>
+    <t>removes 'noise' numbers from the beginning and end of a list</t>
+  </si>
+  <si>
+    <t>calculates the integer part of the value given</t>
+  </si>
+  <si>
+    <t>converts a sequence of numbers, representing ASCII characters, into the Max objects that they represent</t>
+  </si>
+  <si>
+    <t>monitors an arbitrary list, watching for a change in specified elements</t>
+  </si>
+  <si>
+    <t>returns a numeric code corresponding to the value it receives</t>
+  </si>
+  <si>
+    <t>writes it's input to a standard file</t>
+  </si>
+  <si>
+    <t>calculates the greatest common divisor of two numbers</t>
+  </si>
+  <si>
+    <t>an auxiliary object to be used with mtc objects</t>
+  </si>
+  <si>
+    <t>gather n inlets, send out n outlets right-to-left</t>
+  </si>
+  <si>
+    <t>an auxiliary object to be used with x10 objects</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.0</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>shotgun</t>
+  </si>
+  <si>
+    <t>Vsplit</t>
+  </si>
+  <si>
+    <t>senseX</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>gvp100</t>
+  </si>
+  <si>
+    <t>x10units</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>serialX</t>
+  </si>
+  <si>
+    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint server to communicate with one or more tcpClient objects</t>
+  </si>
+  <si>
+    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint server to communicate with a single tcpClient object</t>
+  </si>
+  <si>
+    <t>an interface to the UDP/IP stack on a Macintosh, providing an endpoint to communicate with another udpPort object</t>
+  </si>
+  <si>
+    <t>calculates the absolute value of the input</t>
+  </si>
+  <si>
+    <t>collects a sequence of numbers that are terminated by one of a set of numbers</t>
+  </si>
+  <si>
+    <t>calculates the smallest integer greater than the value given</t>
+  </si>
+  <si>
+    <t>collects atoms into a list</t>
+  </si>
+  <si>
+    <t>calculates the cosine of the input</t>
+  </si>
+  <si>
+    <t>converts a coded representation of a number into the number itself</t>
+  </si>
+  <si>
+    <t>calculates the length of its input list, considered as an n-dimensional vector</t>
+  </si>
+  <si>
+    <t>an implementation of the APL 'drop' operator, which is used to return the remainder of a vector with leading or trailing elements removed</t>
+  </si>
+  <si>
+    <t>converts a number into an encoded representation according to a coding scheme or base</t>
+  </si>
+  <si>
+    <t>calculates the natural exponential of the input</t>
+  </si>
+  <si>
+    <t>calculates the largest integer less than the value given</t>
+  </si>
+  <si>
+    <t>calculates the multiplicative inverse of the input</t>
+  </si>
+  <si>
+    <t>takes as input a list and divides it into a series of fixed-size, shorter, lists. It is similar to the APL 'reshape' operator</t>
+  </si>
+  <si>
+    <t>returns the number of elements in the list that it receives</t>
+  </si>
+  <si>
+    <t>calculates the natural logarithm of the input</t>
+  </si>
+  <si>
+    <t>removes 'noise' numbers from the beginning of a list</t>
+  </si>
+  <si>
+    <t>calculates an arithmetic, geometric, or harmonic mean of the elements of a vector</t>
+  </si>
+  <si>
+    <t>calculates the negative value of the input</t>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0.3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>an interface to Phidget devices (physical widgets)</t>
+  </si>
+  <si>
+    <t>an interface to an ECHOlab DV7 video switcher, which utilizes the Grass Valley Protocol</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>an interface to the Sony Corporation LDP-1550 Laser Disk Player (LDP)</t>
+  </si>
+  <si>
+    <t>an interface to the Macintosh Speech Recognition Manager</t>
+  </si>
+  <si>
+    <t>an interface to the Tactex Controls multi-touch controller (MTC)</t>
+  </si>
+  <si>
+    <t>an interface to the LEGO MINDSTORMS robotic controller</t>
+  </si>
+  <si>
+    <t>an interface to the Labtec six-degrees-of-freedom trackball, the Spaceball</t>
+  </si>
+  <si>
+    <t>an interface to the Macintosh Speech Synthesis Manager, providing control over pitch, rate, volume and voice</t>
+  </si>
+  <si>
+    <t>an interface to the X-10 controller from X-10 Incorporated</t>
+  </si>
+  <si>
+    <t>changes the case of each symbol in a list to either lower case or upper case</t>
+  </si>
+  <si>
+    <t>does a case-sensitive string comparison of two symbols</t>
+  </si>
+  <si>
+    <t>maps its input to a one of a sequence of ranges and returns the set of values associated with the range</t>
+  </si>
+  <si>
+    <t>provides a repository for values, using an associative table to give fast access to the retained data</t>
+  </si>
+  <si>
+    <t>an implementation of a Finite State Machine, with probabilistic transitions</t>
+  </si>
+  <si>
+    <t>an implementation of first-in-first-out queues</t>
+  </si>
+  <si>
+    <t>outputs a pulse when two messages appear within a specified interval</t>
+  </si>
+  <si>
+    <t>an implementation of pushdown stacks, also known as LIFO (last-in, first-out) queues</t>
+  </si>
+  <si>
+    <t>an interface to QuickTime movies, permitting control of playback rate and the section of the movie to be played</t>
+  </si>
+  <si>
+    <t>a windowed interface to QuickTime movies, permitting control of playback rate and the section of the movie to be played</t>
+  </si>
+  <si>
+    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint client to communicate with a tcpServer or a tcpMultiServer object</t>
+  </si>
+  <si>
+    <t>an interface to the TCP/IP stack on a Macintosh, providing a client to identify the IP address corresponding to an Internet address</t>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>N</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>N</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <t>n/a</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
@@ -446,317 +761,6 @@
   <si>
     <t>N</t>
     <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.0.3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>an interface to Phidget devices (physical widgets)</t>
-  </si>
-  <si>
-    <t>an interface to an ECHOlab DV7 video switcher, which utilizes the Grass Valley Protocol</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>an interface to the Sony Corporation LDP-1550 Laser Disk Player (LDP)</t>
-  </si>
-  <si>
-    <t>an interface to the Macintosh Speech Recognition Manager</t>
-  </si>
-  <si>
-    <t>an interface to the Tactex Controls multi-touch controller (MTC)</t>
-  </si>
-  <si>
-    <t>an interface to the LEGO MINDSTORMS robotic controller</t>
-  </si>
-  <si>
-    <t>an interface to the Labtec six-degrees-of-freedom trackball, the Spaceball</t>
-  </si>
-  <si>
-    <t>an interface to the Macintosh Speech Synthesis Manager, providing control over pitch, rate, volume and voice</t>
-  </si>
-  <si>
-    <t>an interface to the X-10 controller from X-10 Incorporated</t>
-  </si>
-  <si>
-    <t>changes the case of each symbol in a list to either lower case or upper case</t>
-  </si>
-  <si>
-    <t>does a case-sensitive string comparison of two symbols</t>
-  </si>
-  <si>
-    <t>maps its input to a one of a sequence of ranges and returns the set of values associated with the range</t>
-  </si>
-  <si>
-    <t>provides a repository for values, using an associative table to give fast access to the retained data</t>
-  </si>
-  <si>
-    <t>an implementation of a Finite State Machine, with probabilistic transitions</t>
-  </si>
-  <si>
-    <t>an implementation of first-in-first-out queues</t>
-  </si>
-  <si>
-    <t>outputs a pulse when two messages appear within a specified interval</t>
-  </si>
-  <si>
-    <t>an implementation of pushdown stacks, also known as LIFO (last-in, first-out) queues</t>
-  </si>
-  <si>
-    <t>an interface to QuickTime movies, permitting control of playback rate and the section of the movie to be played</t>
-  </si>
-  <si>
-    <t>a windowed interface to QuickTime movies, permitting control of playback rate and the section of the movie to be played</t>
-  </si>
-  <si>
-    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint client to communicate with a tcpServer or a tcpMultiServer object</t>
-  </si>
-  <si>
-    <t>an interface to the TCP/IP stack on a Macintosh, providing a client to identify the IP address corresponding to an Internet address</t>
-  </si>
-  <si>
-    <t>gather n inlets, send out n outlets right-to-left</t>
-  </si>
-  <si>
-    <t>an auxiliary object to be used with x10 objects</t>
-  </si>
-  <si>
-    <t>Miscellaneous</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>shotgun</t>
-  </si>
-  <si>
-    <t>Vsplit</t>
-  </si>
-  <si>
-    <t>senseX</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>gvp100</t>
-  </si>
-  <si>
-    <t>x10units</t>
-  </si>
-  <si>
-    <t>changes</t>
-  </si>
-  <si>
-    <t>serialX</t>
-  </si>
-  <si>
-    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint server to communicate with one or more tcpClient objects</t>
-  </si>
-  <si>
-    <t>an interface to the TCP/IP stack on a Macintosh, providing an endpoint server to communicate with a single tcpClient object</t>
-  </si>
-  <si>
-    <t>an interface to the UDP/IP stack on a Macintosh, providing an endpoint to communicate with another udpPort object</t>
-  </si>
-  <si>
-    <t>calculates the absolute value of the input</t>
-  </si>
-  <si>
-    <t>collects a sequence of numbers that are terminated by one of a set of numbers</t>
-  </si>
-  <si>
-    <t>calculates the smallest integer greater than the value given</t>
-  </si>
-  <si>
-    <t>collects atoms into a list</t>
-  </si>
-  <si>
-    <t>calculates the cosine of the input</t>
-  </si>
-  <si>
-    <t>converts a coded representation of a number into the number itself</t>
-  </si>
-  <si>
-    <t>calculates the length of its input list, considered as an n-dimensional vector</t>
-  </si>
-  <si>
-    <t>an implementation of the APL 'drop' operator, which is used to return the remainder of a vector with leading or trailing elements removed</t>
-  </si>
-  <si>
-    <t>converts a number into an encoded representation according to a coding scheme or base</t>
-  </si>
-  <si>
-    <t>calculates the natural exponential of the input</t>
-  </si>
-  <si>
-    <t>calculates the largest integer less than the value given</t>
-  </si>
-  <si>
-    <t>calculates the multiplicative inverse of the input</t>
-  </si>
-  <si>
-    <t>takes as input a list and divides it into a series of fixed-size, shorter, lists. It is similar to the APL 'reshape' operator</t>
-  </si>
-  <si>
-    <t>returns the number of elements in the list that it receives</t>
-  </si>
-  <si>
-    <t>calculates the natural logarithm of the input</t>
-  </si>
-  <si>
-    <t>removes 'noise' numbers from the beginning of a list</t>
-  </si>
-  <si>
-    <t>calculates an arithmetic, geometric, or harmonic mean of the elements of a vector</t>
-  </si>
-  <si>
-    <t>calculates the negative value of the input</t>
-  </si>
-  <si>
-    <t>an implementation of the APL 'reduction' operator, which is used to apply an operator over the elements of a vector</t>
-  </si>
-  <si>
-    <t>redirects a bang to a randomly selected outlet</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>an implementation of the APL 'reverse' operator, which is used to reverse the order of the elements of a vector</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>an interface to the serial ports on a Macintosh; use standard 'serial' object for Max 4.3+</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>[not distributed]</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[not built, doPlügin variant] </t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>(sublist matching)</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of objects defined</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of objects still to be done</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of objects implemented</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.0.1</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>an implementation of the APL 'rotate' operator, which is used to rotate the elements of a vector</t>
-  </si>
-  <si>
-    <t>calculates the integer nearest to the value given</t>
-  </si>
-  <si>
-    <t>removes 'noise' numbers from the end of a list</t>
-  </si>
-  <si>
-    <t>an implementation of the APL 'scan' operator, which is used to apply an operator over the elements of a vector</t>
-  </si>
-  <si>
-    <t>extracts a portion of a list</t>
-  </si>
-  <si>
-    <t>calculates the sine of the input</t>
-  </si>
-  <si>
-    <t>a combination of Vdrop and Vtake</t>
-  </si>
-  <si>
-    <t>calculates the square root of the input</t>
-  </si>
-  <si>
-    <t>an implementation of the APL 'take' operator, which is used to return leading or trailing elements of a vector</t>
-  </si>
-  <si>
-    <t>partitions a list of numbers into a sequence of sublists, separated by 'noise' numbers in the original list</t>
-  </si>
-  <si>
-    <t>removes 'noise' numbers from the beginning and end of a list</t>
-  </si>
-  <si>
-    <t>calculates the integer part of the value given</t>
-  </si>
-  <si>
-    <t>converts a sequence of numbers, representing ASCII characters, into the Max objects that they represent</t>
-  </si>
-  <si>
-    <t>monitors an arbitrary list, watching for a change in specified elements</t>
-  </si>
-  <si>
-    <t>returns a numeric code corresponding to the value it receives</t>
-  </si>
-  <si>
-    <t>writes it's input to a standard file</t>
-  </si>
-  <si>
-    <t>calculates the greatest common divisor of two numbers</t>
-  </si>
-  <si>
-    <t>an auxiliary object to be used with mtc objects</t>
-  </si>
-  <si>
-    <t>provides the logical complement of a number or a list of numbers, returning '0' for each non-zero number and '1' for each zero number</t>
   </si>
 </sst>
 </file>
@@ -832,7 +836,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -858,13 +862,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -880,9 +904,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -894,9 +915,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -916,6 +934,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1249,10 +1282,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="540" topLeftCell="A4" activePane="bottomLeft"/>
-      <selection activeCell="C3" sqref="C1:C1048576"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="540" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1263,21 +1296,21 @@
     <col min="4" max="5" width="3" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="26" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="100.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14" thickBot="1">
       <c r="A1" s="3" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>130</v>
+        <v>227</v>
       </c>
       <c r="D1" s="3">
         <v>3</v>
@@ -1286,20 +1319,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="G1" s="3">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>100</v>
+      <c r="H1" s="3">
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="12" t="s">
-        <v>119</v>
+        <v>197</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1307,92 +1342,101 @@
         <v>17199</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>102</v>
+        <v>198</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K2" t="s">
-        <v>139</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
         <v>17124</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>171</v>
+      <c r="B3" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>1998</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="K3" t="s">
-        <v>140</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
         <v>17120</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>7</v>
+      <c r="B4" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="C4" s="2">
         <v>1996</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>102</v>
+        <v>201</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K4" t="s">
-        <v>143</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1400,60 +1444,66 @@
         <v>17148</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="K5" t="s">
         <v>79</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
         <v>17135</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>23</v>
+      <c r="B6" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="C6" s="2">
         <v>1999</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>0</v>
+        <v>176</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>102</v>
+        <v>203</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K6" t="s">
-        <v>145</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1461,28 +1511,31 @@
         <v>17191</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>166</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>102</v>
+        <v>200</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K7" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1490,31 +1543,34 @@
         <v>17125</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2">
         <v>1998</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>121</v>
+        <v>218</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>107</v>
+        <v>1</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>102</v>
+        <v>204</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K8" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1522,31 +1578,34 @@
         <v>17161</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
       <c r="C9" s="2">
         <v>2001</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>102</v>
+        <v>205</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K9" t="s">
-        <v>147</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1554,28 +1613,31 @@
         <v>17157</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>102</v>
+        <v>206</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K10" t="s">
-        <v>148</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1583,31 +1645,34 @@
         <v>17121</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="C11" s="2">
         <v>1996</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>102</v>
+        <v>207</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>199</v>
       </c>
       <c r="K11" t="s">
-        <v>149</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1615,31 +1680,34 @@
         <v>17146</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2">
         <v>2000</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>127</v>
+        <v>224</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>111</v>
+        <v>202</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K12" t="s">
-        <v>150</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1647,31 +1715,34 @@
         <v>17129</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2">
         <v>1998</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>111</v>
+        <v>205</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K13" t="s">
-        <v>225</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -1679,31 +1750,34 @@
         <v>17186</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="C14" s="2">
         <v>2002</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>111</v>
+      <c r="J14" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K14" t="s">
-        <v>226</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1711,31 +1785,34 @@
         <v>17130</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="C15" s="2">
         <v>1998</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>111</v>
+        <v>205</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K15" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1743,31 +1820,34 @@
         <v>17145</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2">
         <v>2000</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>111</v>
+        <v>205</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K16" t="s">
-        <v>225</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1775,31 +1855,34 @@
         <v>17167</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="C17" s="2">
         <v>2001</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>111</v>
+        <v>202</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K17" t="s">
-        <v>228</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1807,31 +1890,34 @@
         <v>17126</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C18" s="2">
         <v>1998</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>111</v>
+        <v>206</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K18" t="s">
-        <v>229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1839,31 +1925,34 @@
         <v>17204</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>2005</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>132</v>
+        <v>229</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>165</v>
+        <v>1</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>164</v>
+        <v>38</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="K19" t="s">
-        <v>197</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1871,31 +1960,34 @@
         <v>17187</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="C20" s="2">
         <v>2002</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>136</v>
+        <v>176</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>137</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="K20" t="s">
         <v>111</v>
-      </c>
-      <c r="K20" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1903,31 +1995,34 @@
         <v>17122</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2">
         <v>1996</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>111</v>
+        <v>201</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>208</v>
       </c>
       <c r="K21" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1935,31 +2030,34 @@
         <v>17183</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="C22" s="2">
         <v>2001</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" t="s">
         <v>10</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="K22" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1967,31 +2065,34 @@
         <v>17184</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>163</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>135</v>
+        <v>101</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="K23" t="s">
-        <v>205</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1999,31 +2100,34 @@
         <v>17123</v>
       </c>
       <c r="B24" t="s">
-        <v>173</v>
+        <v>46</v>
       </c>
       <c r="C24" s="2">
         <v>1998</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>126</v>
+        <v>223</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>112</v>
+        <v>206</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K24" t="s">
-        <v>224</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -2031,31 +2135,34 @@
         <v>17134</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="C25" s="2">
         <v>1999</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>112</v>
+        <v>205</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K25" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -2063,31 +2170,34 @@
         <v>17153</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="C26" s="2">
         <v>2000</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>141</v>
+        <v>176</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>112</v>
+        <v>201</v>
+      </c>
+      <c r="J26" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K26" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2095,31 +2205,34 @@
         <v>17154</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>139</v>
       </c>
       <c r="C27" s="2">
         <v>2000</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>141</v>
+        <v>176</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>112</v>
+        <v>201</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K27" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -2127,31 +2240,34 @@
         <v>17164</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="C28" s="2">
         <v>2001</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>141</v>
+        <v>176</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>104</v>
+        <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>112</v>
+        <v>201</v>
+      </c>
+      <c r="J28" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K28" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2159,31 +2275,34 @@
         <v>17137</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>122</v>
       </c>
       <c r="C29" s="2">
         <v>2000</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>126</v>
+        <v>176</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>112</v>
+        <v>202</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K29" t="s">
-        <v>153</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -2191,127 +2310,139 @@
         <v>17136</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="C30" s="2">
         <v>2000</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>126</v>
+        <v>176</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>112</v>
+        <v>206</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K30" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31">
         <v>17178</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>63</v>
+      <c r="B31" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="C31" s="2">
         <v>2001</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>112</v>
+        <v>202</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K31" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32">
         <v>17207</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>168</v>
+      <c r="B32" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="C32" s="2">
         <v>2006</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>112</v>
+        <v>210</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K32" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33">
         <v>17138</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>26</v>
+      <c r="B33" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="C33" s="2">
         <v>2000</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>200</v>
+        <v>6</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>112</v>
+        <v>202</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="K33" t="s">
-        <v>157</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -2319,31 +2450,34 @@
         <v>17132</v>
       </c>
       <c r="B34" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="C34" s="2">
         <v>1998</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>114</v>
+        <v>206</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>211</v>
       </c>
       <c r="K34" t="s">
-        <v>158</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -2351,196 +2485,209 @@
         <v>17131</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>117</v>
       </c>
       <c r="C35" s="2">
         <v>1998</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="K35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="18" customFormat="1">
+      <c r="A36" s="18">
+        <v>17127</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="19">
+        <v>1998</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="20" customFormat="1">
+      <c r="A37" s="20">
+        <v>17147</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="17">
+        <v>2000</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="K37" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="18" customFormat="1">
+      <c r="A38" s="18">
+        <v>17144</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="19">
+        <v>2000</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="18" customFormat="1">
+      <c r="A39" s="18">
+        <v>17128</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="K35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="20" customFormat="1">
-      <c r="A36" s="20">
-        <v>17127</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="21">
+      <c r="C39" s="19">
         <v>1998</v>
       </c>
-      <c r="D36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="I36" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="J36" s="21"/>
-      <c r="K36" s="20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="22" customFormat="1">
-      <c r="A37" s="22">
-        <v>17147</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="19">
-        <v>2000</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="I37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="J37" s="19"/>
-      <c r="K37" s="22" t="s">
+      <c r="D39" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="20" customFormat="1">
+      <c r="A40" s="20">
+        <v>17181</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" s="20" customFormat="1">
-      <c r="A38" s="20">
-        <v>17144</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="21">
-        <v>2000</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="J38" s="21"/>
-      <c r="K38" s="20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="20" customFormat="1">
-      <c r="A39" s="20">
-        <v>17128</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="21">
-        <v>1998</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="J39" s="21"/>
-      <c r="K39" s="20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="22" customFormat="1">
-      <c r="A40" s="22">
-        <v>17181</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="19">
+      <c r="C40" s="17">
         <v>2005</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="I40" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="J40" s="19"/>
-      <c r="K40" s="22" t="s">
-        <v>177</v>
+      <c r="D40" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2548,31 +2695,34 @@
         <v>17160</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="C41" s="2">
         <v>2001</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J41" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K41" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2580,31 +2730,34 @@
         <v>17193</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>168</v>
       </c>
       <c r="C42" s="2">
         <v>2003</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J42" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K42" t="s">
-        <v>179</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:11">
@@ -2612,31 +2765,34 @@
         <v>17149</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>134</v>
       </c>
       <c r="C43" s="2">
         <v>2000</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>118</v>
+        <v>200</v>
+      </c>
+      <c r="J43" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K43" t="s">
-        <v>180</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2644,31 +2800,34 @@
         <v>17192</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>167</v>
       </c>
       <c r="C44" s="2">
         <v>2002</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>133</v>
+        <v>230</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>118</v>
+        <v>198</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K44" t="s">
-        <v>181</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="1:11">
@@ -2676,31 +2835,34 @@
         <v>17176</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="C45" s="2">
         <v>2001</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K45" t="s">
-        <v>182</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2708,31 +2870,34 @@
         <v>17166</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>151</v>
       </c>
       <c r="C46" s="2">
         <v>2003</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>136</v>
+        <v>71</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K46" t="s">
-        <v>183</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2740,31 +2905,34 @@
         <v>17163</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="C47" s="2">
         <v>2001</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>127</v>
+        <v>224</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K47" t="s">
-        <v>184</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2772,31 +2940,34 @@
         <v>17140</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="C48" s="2">
         <v>2000</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>118</v>
+        <v>206</v>
+      </c>
+      <c r="J48" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K48" t="s">
-        <v>185</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -2804,31 +2975,34 @@
         <v>17165</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>150</v>
       </c>
       <c r="C49" s="2">
         <v>2003</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K49" t="s">
-        <v>186</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2836,31 +3010,34 @@
         <v>17172</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
       <c r="C50" s="2">
         <v>2001</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>198</v>
+        <v>4</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J50" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K50" t="s">
-        <v>187</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2868,31 +3045,34 @@
         <v>17150</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="C51" s="2">
         <v>2000</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>198</v>
+        <v>4</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>118</v>
+        <v>200</v>
+      </c>
+      <c r="J51" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K51" t="s">
-        <v>188</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2900,31 +3080,34 @@
         <v>17169</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="C52" s="2">
         <v>2001</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J52" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K52" t="s">
-        <v>189</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -2932,31 +3115,34 @@
         <v>17143</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>128</v>
       </c>
       <c r="C53" s="2">
         <v>2000</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J53" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K53" t="s">
-        <v>190</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -2964,31 +3150,34 @@
         <v>17142</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="C54" s="2">
         <v>2000</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J54" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K54" t="s">
-        <v>191</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -2996,31 +3185,34 @@
         <v>17171</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>156</v>
       </c>
       <c r="C55" s="2">
         <v>2001</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K55" t="s">
-        <v>192</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -3028,31 +3220,34 @@
         <v>17194</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="C56" s="2">
         <v>2003</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J56" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K56" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -3060,31 +3255,34 @@
         <v>17162</v>
       </c>
       <c r="B57" t="s">
-        <v>50</v>
+        <v>147</v>
       </c>
       <c r="C57" s="2">
         <v>2001</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J57" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K57" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -3092,31 +3290,34 @@
         <v>17168</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>153</v>
       </c>
       <c r="C58" s="2">
         <v>2001</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J58" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K58" t="s">
-        <v>195</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -3124,31 +3325,34 @@
         <v>17155</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="C59" s="2">
         <v>2000</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J59" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K59" t="s">
-        <v>196</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -3156,31 +3360,34 @@
         <v>17159</v>
       </c>
       <c r="B60" t="s">
-        <v>47</v>
+        <v>144</v>
       </c>
       <c r="C60" s="2">
         <v>2001</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J60" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K60" t="s">
-        <v>201</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -3188,31 +3395,34 @@
         <v>17158</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>143</v>
       </c>
       <c r="C61" s="2">
         <v>2001</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J61" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K61" t="s">
-        <v>211</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -3220,31 +3430,34 @@
         <v>17151</v>
       </c>
       <c r="B62" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="C62" s="2">
         <v>2000</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>118</v>
+        <v>200</v>
+      </c>
+      <c r="J62" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K62" t="s">
-        <v>212</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -3252,31 +3465,34 @@
         <v>17195</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
+        <v>170</v>
       </c>
       <c r="C63" s="2">
         <v>2003</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J63" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K63" t="s">
-        <v>213</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -3284,31 +3500,34 @@
         <v>17156</v>
       </c>
       <c r="B64" t="s">
-        <v>44</v>
+        <v>141</v>
       </c>
       <c r="C64" s="2">
         <v>2000</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J64" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K64" t="s">
-        <v>214</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -3316,31 +3535,34 @@
         <v>17141</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>126</v>
       </c>
       <c r="C65" s="2">
         <v>2000</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>118</v>
+        <v>206</v>
+      </c>
+      <c r="J65" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K65" t="s">
-        <v>215</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -3348,31 +3570,34 @@
         <v>17177</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>159</v>
       </c>
       <c r="C66" s="2">
         <v>2001</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J66" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K66" t="s">
-        <v>216</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -3380,31 +3605,34 @@
         <v>17205</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>40</v>
       </c>
       <c r="C67" s="2">
         <v>2005</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J67" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K67" t="s">
-        <v>217</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -3412,31 +3640,34 @@
         <v>17170</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>155</v>
       </c>
       <c r="C68" s="2">
         <v>2001</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>118</v>
+        <v>202</v>
+      </c>
+      <c r="J68" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K68" t="s">
-        <v>218</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -3444,31 +3675,34 @@
         <v>17139</v>
       </c>
       <c r="B69" t="s">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="C69" s="2">
         <v>2000</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>142</v>
+        <v>77</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>118</v>
+        <v>206</v>
+      </c>
+      <c r="J69" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K69" t="s">
-        <v>219</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -3476,31 +3710,34 @@
         <v>17197</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>172</v>
       </c>
       <c r="C70" s="2">
         <v>2003</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J70" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K70" t="s">
-        <v>220</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -3508,31 +3745,34 @@
         <v>17196</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
       <c r="C71" s="2">
         <v>2003</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J71" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K71" t="s">
-        <v>221</v>
+        <v>27</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -3540,31 +3780,34 @@
         <v>17152</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="C72" s="2">
         <v>2000</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>118</v>
+        <v>200</v>
+      </c>
+      <c r="J72" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K72" t="s">
-        <v>222</v>
+        <v>28</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -3572,31 +3815,34 @@
         <v>17198</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>173</v>
       </c>
       <c r="C73" s="2">
         <v>2003</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>141</v>
+        <v>76</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>118</v>
+        <v>210</v>
+      </c>
+      <c r="J73" s="22" t="s">
+        <v>215</v>
       </c>
       <c r="K73" t="s">
-        <v>223</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="1:11" s="4" customFormat="1">
@@ -3604,48 +3850,54 @@
         <v>17202</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H74" s="5"/>
-      <c r="J74" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I74" s="5"/>
+      <c r="J74" s="25"/>
     </row>
     <row r="75" spans="1:11" s="4" customFormat="1">
       <c r="A75" s="4">
         <v>17188</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>89</v>
+        <v>186</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H75" s="5"/>
-      <c r="J75" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I75" s="5"/>
+      <c r="J75" s="25"/>
       <c r="K75" s="4" t="s">
-        <v>123</v>
+        <v>220</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="4" customFormat="1">
@@ -3653,25 +3905,28 @@
         <v>17208</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H76" s="5"/>
-      <c r="J76" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I76" s="5"/>
+      <c r="J76" s="25"/>
       <c r="K76" s="4" t="s">
-        <v>125</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="4" customFormat="1">
@@ -3679,25 +3934,28 @@
         <v>17133</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H77" s="5"/>
-      <c r="J77" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="25"/>
       <c r="K77" s="4" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="4" customFormat="1">
@@ -3705,25 +3963,28 @@
         <v>17200</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>92</v>
+        <v>189</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H78" s="5"/>
-      <c r="J78" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I78" s="5"/>
+      <c r="J78" s="25"/>
       <c r="K78" s="4" t="s">
-        <v>122</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="4" customFormat="1">
@@ -3731,94 +3992,106 @@
         <v>17209</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H79" s="5"/>
-      <c r="J79" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="J79" s="25"/>
     </row>
     <row r="80" spans="1:11" s="4" customFormat="1">
       <c r="A80" s="4">
         <v>17201</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H80" s="5"/>
-      <c r="J80" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="J80" s="25"/>
     </row>
     <row r="81" spans="1:14" s="4" customFormat="1">
       <c r="A81" s="4">
         <v>17190</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>91</v>
+        <v>188</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H81" s="5"/>
-      <c r="J81" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I81" s="5"/>
+      <c r="J81" s="25"/>
     </row>
     <row r="82" spans="1:14" s="4" customFormat="1">
       <c r="A82" s="4">
         <v>17203</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G82" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="11" t="s">
-        <v>162</v>
+        <v>177</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I82" s="5"/>
+      <c r="J82" s="25"/>
+      <c r="K82" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="83" spans="1:14" s="4" customFormat="1">
@@ -3826,94 +4099,106 @@
         <v>17182</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>87</v>
+        <v>184</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H83" s="5"/>
-      <c r="J83" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I83" s="5"/>
+      <c r="J83" s="25"/>
     </row>
     <row r="84" spans="1:14" s="4" customFormat="1">
       <c r="A84" s="4">
         <v>17179</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="J84" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H84" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I84" s="5"/>
+      <c r="J84" s="25"/>
     </row>
     <row r="85" spans="1:14" s="4" customFormat="1">
       <c r="A85" s="4">
         <v>17174</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H85" s="5"/>
-      <c r="J85" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="25"/>
     </row>
     <row r="86" spans="1:14" s="4" customFormat="1">
       <c r="A86" s="4">
         <v>17206</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="C86" s="5"/>
       <c r="D86" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="11" t="s">
-        <v>206</v>
+        <v>177</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I86" s="5"/>
+      <c r="J86" s="25"/>
+      <c r="K86" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:14" s="4" customFormat="1">
@@ -3921,144 +4206,163 @@
         <v>17175</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H87" s="5"/>
-      <c r="J87" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H87" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I87" s="5"/>
+      <c r="J87" s="25"/>
     </row>
     <row r="88" spans="1:14" s="4" customFormat="1">
       <c r="A88" s="4">
         <v>17173</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H88" s="5"/>
-      <c r="J88" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="J88" s="25"/>
     </row>
     <row r="89" spans="1:14" s="4" customFormat="1">
       <c r="A89" s="4">
         <v>17180</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>86</v>
+        <v>183</v>
       </c>
       <c r="C89" s="5"/>
       <c r="D89" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H89" s="5"/>
-      <c r="J89" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I89" s="5"/>
+      <c r="J89" s="25"/>
     </row>
     <row r="90" spans="1:14" s="4" customFormat="1">
       <c r="A90" s="4">
         <v>17185</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>88</v>
+        <v>185</v>
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H90" s="5"/>
-      <c r="J90" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H90" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I90" s="5"/>
+      <c r="J90" s="25"/>
     </row>
     <row r="91" spans="1:14" s="4" customFormat="1">
       <c r="A91" s="4">
         <v>17189</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>90</v>
+        <v>187</v>
       </c>
       <c r="C91" s="5"/>
       <c r="D91" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H91" s="5"/>
-      <c r="J91" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I91" s="5"/>
+      <c r="J91" s="25"/>
       <c r="K91" s="4" t="s">
-        <v>124</v>
+        <v>221</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="14" thickBot="1"/>
     <row r="93" spans="1:14" s="6" customFormat="1">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8">
         <f>COUNTIF(D2:D92,"Y")</f>
         <v>56</v>
       </c>
-      <c r="E93" s="9">
-        <f t="shared" ref="E93:G93" si="0">COUNTIF(E2:E92,"Y")</f>
+      <c r="E93" s="8">
+        <f t="shared" ref="E93:H93" si="0">COUNTIF(E2:E92,"Y")</f>
         <v>72</v>
       </c>
-      <c r="F93" s="9">
+      <c r="F93" s="8">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="G93" s="9">
+      <c r="G93" s="8">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H93" s="10"/>
-      <c r="J93" s="7"/>
+      <c r="H93" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I93" s="9"/>
+      <c r="J93" s="27"/>
     </row>
     <row r="94" spans="1:14">
       <c r="D94"/>
@@ -4066,12 +4370,9 @@
       <c r="F94"/>
       <c r="G94"/>
       <c r="H94"/>
-      <c r="J94" s="2">
-        <f>COUNT(A2:A92)</f>
-        <v>90</v>
-      </c>
+      <c r="I94"/>
       <c r="K94" s="1" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
@@ -4083,12 +4384,9 @@
       <c r="F95"/>
       <c r="G95"/>
       <c r="H95"/>
-      <c r="J95" s="2">
-        <f>J94-J96</f>
-        <v>18</v>
-      </c>
+      <c r="I95"/>
       <c r="K95" s="1" t="s">
-        <v>208</v>
+        <v>14</v>
       </c>
       <c r="L95" s="2"/>
       <c r="M95" s="2"/>
@@ -4100,12 +4398,9 @@
       <c r="F96"/>
       <c r="G96"/>
       <c r="H96"/>
-      <c r="J96" s="2">
-        <f>MAX(D93:G93)</f>
-        <v>72</v>
-      </c>
+      <c r="I96"/>
       <c r="K96" s="1" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
       <c r="L96" s="2"/>
       <c r="M96" s="2"/>
@@ -4119,6 +4414,7 @@
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>